<commit_message>
Added Joint Rate Comparisons for res/com/ind, 2017-2023, with PDFs
</commit_message>
<xml_diff>
--- a/Fig6_ResRateTimeSeries/Jan1BaselineTieredRate.xlsx
+++ b/Fig6_ResRateTimeSeries/Jan1BaselineTieredRate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rayan/Developer/CCAResearch/ConsolidatedPrimerData/CA_electricity_primer/Fig6_ResRateTimeSeries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5796E2B7-1313-9846-BF94-197A27B31066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5015AA3B-8DD2-FB41-B9B6-9CEDD03DB1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14260" activeTab="2" xr2:uid="{2ED96552-DAFC-C646-85A2-7A03F356D192}"/>
+    <workbookView xWindow="1600" yWindow="500" windowWidth="25600" windowHeight="14260" activeTab="2" xr2:uid="{2ED96552-DAFC-C646-85A2-7A03F356D192}"/>
   </bookViews>
   <sheets>
     <sheet name="residential" sheetId="1" r:id="rId1"/>
@@ -6691,14 +6691,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>301796</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:colOff>200196</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>14475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>381001</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:colOff>279401</xdr:colOff>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>94772</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7170,7 +7170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C765326C-66C9-9B4E-AA2F-2EFB2434479E}">
   <dimension ref="A1:R142"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="194" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
@@ -10711,7 +10711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9456EBFD-B61B-F549-B6C4-33D3AA6702D9}">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView zoomScale="181" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="181" workbookViewId="0">
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
@@ -12209,9 +12209,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C73EA71-FD44-AA49-B897-B390D8FC9C19}">
   <dimension ref="A1:Q83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA10" sqref="AA10"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="139" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X35" sqref="X35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>